<commit_message>
Final Changes have been made
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca Szilagyi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38064076-DF88-4A6B-8AE6-622484943BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F3F22D-B92E-424F-A550-961B33B51D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2487EDBD-1BE8-41D7-BF4E-DEC25DB216EF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>Piesa</t>
   </si>
@@ -102,9 +102,6 @@
     <t xml:space="preserve">Senzori de Limita </t>
   </si>
   <si>
-    <t>Cate Unul pentru fiecare axa, cel de pe Axa Y nu va fi prea folosit.</t>
-  </si>
-  <si>
     <t>Unul Integrat in Placa de control, altul pentru Hotend, iar unul pentru Pat *.</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>Piulita Trapeizoidala T8</t>
   </si>
   <si>
-    <t>* - componente necesare doar daca se opteaza pentru un pat incalzit</t>
-  </si>
-  <si>
     <t>Componente necesare pentru alte componente electronice</t>
   </si>
   <si>
@@ -157,6 +151,30 @@
   </si>
   <si>
     <t>Necesar</t>
+  </si>
+  <si>
+    <t>Cate Unul pentru fiecare axa ( X și Z)</t>
+  </si>
+  <si>
+    <t>cate este cazul</t>
+  </si>
+  <si>
+    <t>Rulment Axial 51103</t>
+  </si>
+  <si>
+    <t>1 sau 3</t>
+  </si>
+  <si>
+    <t>3 în cazul în care se va implementa un pat incălzit (incă în lucru)</t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Unelte,conectori,zip-ties,cabluri USB, etc</t>
   </si>
 </sst>
 </file>
@@ -199,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -209,6 +227,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -524,16 +545,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC2240D6-167B-44D4-B061-AB87214873FC}">
-  <dimension ref="A1:C98"/>
+  <dimension ref="A1:C99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="62.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -623,13 +644,17 @@
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -643,13 +668,17 @@
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -659,23 +688,23 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="2">
-        <v>1</v>
+        <v>41</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
@@ -686,10 +715,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B18" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C18" t="s">
         <v>23</v>
@@ -697,7 +726,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B19" s="2">
         <v>3</v>
@@ -708,23 +737,26 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B20" s="2">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B21" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B22" s="2">
         <v>1</v>
@@ -732,26 +764,26 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B23" s="2">
         <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B24" s="2">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B25" s="2">
         <v>2</v>
@@ -759,44 +791,52 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B26" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" t="s">
+      <c r="A28" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B30" s="2">
+      <c r="B31" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
@@ -994,52 +1034,53 @@
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B81" s="2"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
@@ -1047,6 +1088,9 @@
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>